<commit_message>
atualizações relatório comentários AAA
</commit_message>
<xml_diff>
--- a/inst/da_arbitragem.xlsx
+++ b/inst/da_arbitragem.xlsx
@@ -561,7 +561,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -841,7 +841,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1350,7 +1350,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1462,7 +1462,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1630,7 +1630,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2887,7 +2887,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3742,7 +3742,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4327,7 +4327,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -4841,7 +4841,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -4897,7 +4897,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -5650,7 +5650,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -5706,7 +5706,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -5818,7 +5818,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -5874,7 +5874,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -5930,7 +5930,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -5986,7 +5986,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -6617,7 +6617,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -6729,7 +6729,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -6785,7 +6785,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -6897,7 +6897,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -8215,7 +8215,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -8612,7 +8612,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -9243,7 +9243,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -9589,7 +9589,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -10337,7 +10337,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -11080,7 +11080,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -11696,7 +11696,7 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -12037,7 +12037,7 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -12093,7 +12093,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -12149,7 +12149,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -12205,7 +12205,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -12261,7 +12261,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -12378,7 +12378,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -12724,7 +12724,7 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -13121,7 +13121,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -13574,7 +13574,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -13686,7 +13686,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -14256,7 +14256,7 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -15605,7 +15605,7 @@
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -15890,7 +15890,7 @@
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -16348,7 +16348,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">

</xml_diff>